<commit_message>
farto desta porra tirem me desta cadeira
</commit_message>
<xml_diff>
--- a/Programa projeto/Grid_independency.xlsx
+++ b/Programa projeto/Grid_independency.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Farinha\Documents\GitHub\TCal\Programa projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A996DAE-26BD-494C-8FCB-799F194B4F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3A4C37-8674-43D0-8C30-2C823583C8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Folha8" sheetId="8" r:id="rId8"/>
     <sheet name="Folha9" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="5">
   <si>
     <t>Mesh 12x12</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Mesh 82x82</t>
+  </si>
+  <si>
+    <t>Mesh 62x62</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -87,12 +90,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,25 +464,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8702A7-9CA3-494A-BF6E-176C30307FCA}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -436,10 +495,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>979.06710023338542</v>
       </c>
@@ -458,14 +520,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>980.84227605763385</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>978.67099901486949</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>978.70513028530706</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>895.29517170522251</v>
       </c>
@@ -484,14 +552,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>898.6199608972131</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>895.01128819594737</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>895.02931452389521</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>610.98914236724352</v>
       </c>
@@ -510,14 +584,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>619.3868105259927</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>610.85371216846488</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>610.85978964449396</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>393.33964435553355</v>
       </c>
@@ -536,14 +616,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>403.7029223226649</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>393.15515992671351</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>393.15744204126622</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>170.12760243527299</v>
       </c>
@@ -562,14 +648,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>178.40749829988408</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>169.98578259819405</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>169.98576758454647</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>80.43951192031335</v>
       </c>
@@ -588,14 +680,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>85.406947215667813</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>80.417372886713537</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>80.417794441738721</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>44.405728774370296</v>
       </c>
@@ -614,14 +712,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>47.006737921166987</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>44.460613608226524</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>44.461961911375809</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>29.918368250795979</v>
       </c>
@@ -640,10 +744,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>31.1511685604086</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>30.026087024489271</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>30.027805567205121</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>
@@ -654,25 +764,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE08FCC8-59D8-479C-81D2-3B7E7E91E909}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E11"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -683,10 +795,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1055.7327882315753</v>
       </c>
@@ -705,14 +820,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>1057.4546054398556</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>1055.7519972824962</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1055.7784835114903</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>996.55739515569303</v>
       </c>
@@ -731,14 +852,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>999.95827581035746</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>996.68929380229656</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>996.71021921788804</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>711.5495208084086</v>
       </c>
@@ -757,14 +884,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>721.30565910433552</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>711.49664186623477</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>711.50725388607748</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>458.58927823803396</v>
       </c>
@@ -783,14 +916,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>470.78027920260791</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>458.39533395019987</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>458.39989638162433</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>196.39361447019647</v>
       </c>
@@ -809,14 +948,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>206.13096439336573</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>196.2346031880395</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>196.23532621422689</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>91.01389937953769</v>
       </c>
@@ -835,14 +980,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>96.854072674150757</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>90.990955062666842</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>90.991748717261757</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>48.675710855417684</v>
       </c>
@@ -861,14 +1012,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>51.733292686870968</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>48.741440420788734</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>48.743145462618315</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>31.653667987010049</v>
       </c>
@@ -887,10 +1044,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>33.1027781571118</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>31.780742211715793</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>31.782811014846779</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>
@@ -901,25 +1064,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7C50E1-1AE2-456B-B094-FEC273A208B3}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -930,10 +1095,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1059.8466210671231</v>
       </c>
@@ -952,14 +1120,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>1061.090042172953</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>1059.7106667427374</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1059.7332039628141</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1009.0707467018613</v>
       </c>
@@ -978,14 +1152,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>1011.9874797828243</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>1009.1617741541788</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>1009.1799177276201</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>739.92800998482778</v>
       </c>
@@ -1004,14 +1184,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>750.01603721975766</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>739.92992155115962</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>739.94302130769972</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>477.80707577564408</v>
       </c>
@@ -1030,14 +1216,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>490.53342613581367</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>477.61069084952254</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>477.61661926975114</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>204.14230616491568</v>
       </c>
@@ -1056,14 +1248,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>214.30932268284249</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>203.97767564137405</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>203.97888973390224</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>94.133439033884514</v>
       </c>
@@ -1082,14 +1280,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>100.23095742974999</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>94.110035747197657</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>94.111049265413385</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>49.935394078147397</v>
       </c>
@@ -1108,14 +1312,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>53.127619224264549</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>50.004233307487496</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>50.006088154628131</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>32.165597058991487</v>
       </c>
@@ -1134,10 +1344,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>33.678500048896296</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>32.298344585219454</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>32.300534978454451</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>
@@ -1148,25 +1364,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611528C6-78EF-4DD4-B02C-4540478A9A9F}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1177,10 +1395,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1031.2291864533158</v>
       </c>
@@ -1199,14 +1420,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>1033.5518146449845</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>1031.3206575452123</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1031.3564098115849</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>952.27115808814392</v>
       </c>
@@ -1225,14 +1452,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>956.03025330444302</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>952.22360822082169</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>952.246848903814</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>651.76342574689477</v>
       </c>
@@ -1251,14 +1484,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>660.73803234259708</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>651.65067710574795</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>651.65982328889254</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>419.09677246967811</v>
       </c>
@@ -1277,14 +1516,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>430.17301361375758</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>418.92033067412348</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>418.92459596345986</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>180.48073877772208</v>
       </c>
@@ -1303,14 +1548,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>189.33535977028399</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>180.34100247026785</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>180.34193193072053</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>84.60532259315292</v>
       </c>
@@ -1329,14 +1580,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>89.9190950907348</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>84.587977760607401</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>84.588984913685863</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>46.085590688379305</v>
       </c>
@@ -1355,14 +1612,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>48.869818225487478</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>46.148566324931537</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>46.150372694908221</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>30.599776788518177</v>
       </c>
@@ -1381,10 +1644,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>31.920440383451503</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>30.717519413978867</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>30.719615037448754</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>
@@ -1395,25 +1664,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF84E56E-23EA-4AE0-8D3E-62656AC16B54}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1424,10 +1695,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1112.3241891173029</v>
       </c>
@@ -1446,14 +1720,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>1114.6228963518945</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>1112.8990120091707</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1112.9236859424047</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1060.1953243844187</v>
       </c>
@@ -1472,14 +1752,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>1064.0642642642047</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>1060.622521911245</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>1060.6467746443745</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>759.26193142626016</v>
       </c>
@@ -1498,14 +1784,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>769.69096310141038</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>759.24568702924955</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>759.25885248288705</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>488.8480572993634</v>
       </c>
@@ -1524,14 +1816,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>501.87883104563616</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>488.66692231550826</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>488.67316062188536</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>208.55811395030608</v>
       </c>
@@ -1550,14 +1848,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>218.97177828216238</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>208.40279624103229</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>208.40436543479126</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>95.908552737193418</v>
       </c>
@@ -1576,14 +1880,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>102.15608592761205</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>95.891743058361641</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>95.893118557390352</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>50.649478365844949</v>
       </c>
@@ -1602,14 +1912,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>53.922510935776835</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>50.724917431872321</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>50.727117652630291</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>32.454294527720648</v>
       </c>
@@ -1628,10 +1944,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>34.006713381734301</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>32.593229662007516</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>32.595723859542552</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>
@@ -1642,25 +1964,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE21D5CA-FACC-4C6E-A797-421E13966021}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1671,10 +1995,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1116.7009128379534</v>
       </c>
@@ -1693,14 +2020,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>1118.4931338848473</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>1117.1131815978792</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1117.133452340388</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1073.5493415982805</v>
       </c>
@@ -1719,14 +2052,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>1076.9073187023996</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>1073.9366021794099</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>1073.957415486318</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>789.59844782713776</v>
       </c>
@@ -1745,14 +2084,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>800.38399333776715</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>789.64418616361399</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>789.65928003824683</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>509.39171579987192</v>
       </c>
@@ -1771,14 +2116,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>522.99544382977888</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>509.21034093127753</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>509.21756371318361</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>216.84117281807534</v>
       </c>
@@ -1797,14 +2148,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>227.7146389518231</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>216.68098532967778</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>216.68289881826453</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>99.2431075558586</v>
       </c>
@@ -1823,14 +2180,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>105.76605651280606</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>99.226344904616013</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>99.227891694454371</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>51.995866390104801</v>
       </c>
@@ -1849,14 +2212,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>55.413079359169323</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>52.074937445158668</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>52.077279183843338</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>33.001393985751065</v>
       </c>
@@ -1875,10 +2244,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>34.622173856404594</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>33.146562757793106</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>33.149184899513649</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>
@@ -1889,25 +2264,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A353961B-18C0-4C13-847E-9140040D0BF9}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1918,10 +2295,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1047.6135515299864</v>
       </c>
@@ -1940,14 +2320,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>1050.0713165319366</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>1047.8530651666802</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1047.8869903046011</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>975.14585051961319</v>
       </c>
@@ -1966,14 +2352,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>979.14156380081567</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>975.29522923417937</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>975.32227227923988</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>669.49731362494128</v>
       </c>
@@ -1992,14 +2384,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>678.66166780158346</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>669.39952857383059</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>669.41171981176967</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>430.2976221360147</v>
       </c>
@@ -2018,14 +2416,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>441.64430328360754</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>430.12873906028278</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>430.13520110799948</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>184.97636356799626</v>
       </c>
@@ -2044,14 +2448,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>194.07111332207512</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>184.84431069340488</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>184.84655503024896</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>86.410491731236519</v>
       </c>
@@ -2070,14 +2480,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>91.874502398992846</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>86.400465414348986</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>86.402404512010548</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>46.808728854315589</v>
       </c>
@@ -2096,14 +2512,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>49.677212163760011</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>46.881109654012278</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>46.883643362384404</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>30.890701071145219</v>
       </c>
@@ -2122,10 +2544,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>32.253815925755532</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>31.016794528493456</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>31.019468685530889</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>
@@ -2136,25 +2564,27 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3A46A2-EC4C-42BB-B0D7-603977F6C887}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2165,10 +2595,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1130.2126707191892</v>
       </c>
@@ -2187,14 +2620,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>1132.6657573839966</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>1130.9639355048605</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1130.9848987786322</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1085.7848777070622</v>
       </c>
@@ -2213,14 +2652,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>1089.9240000700818</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>1086.4457457910441</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>1086.4721521890333</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>780.01356694149911</v>
       </c>
@@ -2239,14 +2684,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>790.66639951110892</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>780.02064286419886</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>780.0362376163921</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>502.00651865816565</v>
       </c>
@@ -2265,14 +2716,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>515.35655186546899</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>501.83666830972311</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>501.84478840131464</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>213.84028388727288</v>
       </c>
@@ -2291,14 +2748,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>224.53676539930342</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>213.69491574406567</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>213.69774895355363</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>98.029550995834029</v>
       </c>
@@ -2317,14 +2780,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>104.45388693287362</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>98.021711548213261</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>98.024068864295117</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>51.499135474903895</v>
       </c>
@@ -2343,14 +2812,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>54.871280328178486</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>51.585775525545408</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>51.588784499594411</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>32.796118395656066</v>
       </c>
@@ -2369,10 +2844,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>34.398463301717968</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>32.944927015710746</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>32.94808216383052</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>
@@ -2383,25 +2864,27 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D795DC60-46CD-4C58-96AA-228AD02DECE4}">
-  <dimension ref="D2:N11"/>
+  <dimension ref="D2:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.140625" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.140625" customWidth="true"/>
+    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="11" max="11" width="5.140625" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="5.140625" customWidth="true"/>
+    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="17" max="17" width="5.140625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -2412,10 +2895,13 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1134.6923189111512</v>
       </c>
@@ -2434,14 +2920,20 @@
       <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4">
-        <v>1136.6325397385649</v>
-      </c>
-      <c r="N4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="0">
+        <v>1135.2790627298302</v>
+      </c>
+      <c r="N4" s="0">
+        <v>60</v>
+      </c>
+      <c r="P4" s="0">
+        <v>1135.2953441525888</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1099.4918476774369</v>
       </c>
@@ -2460,14 +2952,20 @@
       <c r="K5">
         <v>120</v>
       </c>
-      <c r="M5">
-        <v>1103.1173535496755</v>
-      </c>
-      <c r="N5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="0">
+        <v>1100.1145938081133</v>
+      </c>
+      <c r="N5" s="0">
+        <v>120</v>
+      </c>
+      <c r="P5" s="0">
+        <v>1100.1370351216624</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>811.20180458585139</v>
       </c>
@@ -2486,14 +2984,20 @@
       <c r="K6">
         <v>500</v>
       </c>
-      <c r="M6">
-        <v>822.22089790038308</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="0">
+        <v>811.27517951577556</v>
+      </c>
+      <c r="N6" s="0">
+        <v>500</v>
+      </c>
+      <c r="P6" s="0">
+        <v>811.29208292819521</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>523.12675052104817</v>
       </c>
@@ -2512,14 +3016,20 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="M7">
-        <v>537.06448765247353</v>
-      </c>
-      <c r="N7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="0">
+        <v>522.95851183874231</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="0">
+        <v>522.96721780759913</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>222.35538011248968</v>
       </c>
@@ -2538,14 +3048,20 @@
       <c r="K8">
         <v>2000</v>
       </c>
-      <c r="M8">
-        <v>233.52442705044746</v>
-      </c>
-      <c r="N8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="0">
+        <v>222.2060951480305</v>
+      </c>
+      <c r="N8" s="0">
+        <v>2000</v>
+      </c>
+      <c r="P8" s="0">
+        <v>222.20913421304647</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>101.45727825304152</v>
       </c>
@@ -2564,14 +3080,20 @@
       <c r="K9">
         <v>3000</v>
       </c>
-      <c r="M9">
-        <v>108.16493704442757</v>
-      </c>
-      <c r="N9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="0">
+        <v>101.45008769099826</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3000</v>
+      </c>
+      <c r="P9" s="0">
+        <v>101.45258126829361</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>52.882847728395632</v>
       </c>
@@ -2590,14 +3112,20 @@
       <c r="K10">
         <v>4000</v>
       </c>
-      <c r="M10">
-        <v>56.403584811922372</v>
-      </c>
-      <c r="N10">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="0">
+        <v>52.973695973182842</v>
+      </c>
+      <c r="N10" s="0">
+        <v>4000</v>
+      </c>
+      <c r="P10" s="0">
+        <v>52.976850328343986</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>33.358233690390293</v>
       </c>
@@ -2616,10 +3144,16 @@
       <c r="K11">
         <v>5000</v>
       </c>
-      <c r="M11">
-        <v>35.031156729342015</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="0">
+        <v>33.513744196397177</v>
+      </c>
+      <c r="N11" s="0">
+        <v>5000</v>
+      </c>
+      <c r="P11" s="0">
+        <v>33.517043328418907</v>
+      </c>
+      <c r="Q11" s="0">
         <v>5000</v>
       </c>
     </row>

</xml_diff>